<commit_message>
add new notebooks for experimental datasets
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zsailer/Documents/Research/projects/notebooks/epistasis-paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zsailer/Documents/Research/projects/notebooks/epistasis-notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Dataset</t>
   </si>
@@ -107,10 +107,19 @@
     <t>hormone sensitivity to drug</t>
   </si>
   <si>
-    <t>Signficant Order (linear epistasis)</t>
-  </si>
-  <si>
     <t>Non-Linear fit success</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Significant Order (linear epistasis)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -437,7 +446,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,10 +471,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -484,6 +493,9 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -495,6 +507,9 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -506,6 +521,9 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -517,6 +535,9 @@
       <c r="C5" t="s">
         <v>25</v>
       </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -528,6 +549,9 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -539,6 +563,9 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -550,6 +577,9 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -561,6 +591,9 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -572,6 +605,9 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -583,6 +619,9 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -594,6 +633,9 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -604,6 +646,9 @@
       </c>
       <c r="C13" t="s">
         <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add lattice protein analysis
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Dataset</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Non-linear score</t>
   </si>
 </sst>
 </file>
@@ -163,9 +166,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,13 +463,14 @@
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -470,20 +480,23 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -493,11 +506,14 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -507,11 +523,11 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -521,11 +537,11 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -535,11 +551,11 @@
       <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -549,11 +565,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -563,11 +579,11 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -577,11 +593,11 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -591,11 +607,11 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -605,11 +621,14 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -619,11 +638,11 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -633,11 +652,11 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -647,8 +666,14 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="F13">
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>